<commit_message>
Added consolidated prod details
</commit_message>
<xml_diff>
--- a/Hudson_Advisor_Capital_Market_BCP_Data.xlsx
+++ b/Hudson_Advisor_Capital_Market_BCP_Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HudSon_Packages_Mine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Huds0n_Capital Market\Github\Huds0nCapitalMarket\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="88">
   <si>
     <t>Job Name</t>
   </si>
@@ -252,6 +252,42 @@
   </si>
   <si>
     <t>'G:\LossMit\Processing</t>
+  </si>
+  <si>
+    <t>Hudson_Daily_NQM_AMC_SFTP_ETL</t>
+  </si>
+  <si>
+    <t>C:\SSIS\Daily_Feed\Daily_AMC_SFTP_DataLoad.dtsx</t>
+  </si>
+  <si>
+    <t>Daily_AMC_SFTP_DataLoad</t>
+  </si>
+  <si>
+    <t>Doesn’t have BCp, Excel to DB</t>
+  </si>
+  <si>
+    <t>C:\SSIS\Daily_Feed\Daily_CHL_SFTP_Data_Download.dtsx</t>
+  </si>
+  <si>
+    <t>Daily_CHL_SFTP_Data_Download</t>
+  </si>
+  <si>
+    <t>Hudson_Daily_NQM_CHL_SFTP_ETL</t>
+  </si>
+  <si>
+    <t>Hudson_Daily_NQM_CHL_SFTP_UPLOAD_ETL</t>
+  </si>
+  <si>
+    <t>C:\SSIS\Daily_Feed\Daily_CHL_SFTP_Data_Upload.dtsx</t>
+  </si>
+  <si>
+    <t>Daily_CHL_SFTP_Data_Upload</t>
+  </si>
+  <si>
+    <t>Doesn’t have BCP, generates txt and uploades to SFTP</t>
+  </si>
+  <si>
+    <t>Hudson_Daily_NQM_ETL</t>
   </si>
 </sst>
 </file>
@@ -318,9 +354,6 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -331,6 +364,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -616,405 +652,497 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="72.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="49.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="41.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="42.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="72.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="49.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="3" t="s">
+      <c r="H3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="3" t="s">
+      <c r="H4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="3" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="3" t="s">
+      <c r="H8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="3" t="s">
+      <c r="H9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="3" t="s">
+      <c r="H10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="3" t="s">
+      <c r="H11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="3" t="s">
+      <c r="H12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>16</v>
+      <c r="H13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>